<commit_message>
dossier tests + rapport
</commit_message>
<xml_diff>
--- a/Compil/cahier_test_Capodano_Hamel.xlsx
+++ b/Compil/cahier_test_Capodano_Hamel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GITrepos\Compil\Compil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C248BE-89A0-4372-A4CF-C59F73462FFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3357E722-F510-4A6F-91A0-BA19A0ED16D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{57553EF0-D143-41F5-A1D1-F73F5D42473B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>But du test</t>
   </si>
@@ -1762,6 +1762,400 @@
 3
 4
 5</t>
+  </si>
+  <si>
+    <t>#include&lt;stdlib&gt;
+#include&lt;stdio&gt;
+function main()
+{
+	var i = 0;
+	var j = 10;
+	while (i &lt; 5)
+	{
+		while (j &gt; 7)
+		{
+			print(j);
+			j = j - 1;
+		}
+		print(i);
+		i = i + 1;
+	}
+	return 0;
+}</t>
+  </si>
+  <si>
+    <t>resn 0
+.pow
+resn 2
+get 0
+dup
+set 3
+get 1
+push 1
+sub
+dup
+set 2
+.loop0
+get 2
+push 0
+cmpgt
+jumpf l0
+get 3
+get 0
+mul
+dup
+set 3
+drop
+get 2
+push 1
+sub
+dup
+set 2
+jump l1
+.l0
+jump loop1
+.l1
+jump loop0
+.loop1
+get 3
+ret
+push 0
+ret
+.printx
+resn 1
+get 0
+push 0
+cmpne
+jumpf l2
+prep printx
+get 0
+push 10
+div
+call 1
+drop
+get 0
+push 10
+mod
+push 48
+add
+dup
+set 1
+drop
+get 1
+dup
+send
+.l2
+push 0
+ret
+.print
+resn 0
+get 0
+push 0
+cmpeq
+jumpf l4
+push 48
+dup
+send
+jump l5
+.l4
+get 0
+push 0
+cmplt
+jumpf l6
+push 45
+dup
+send
+prep printx
+push 0
+get 0
+sub
+call 1
+drop
+jump l7
+.l6
+prep printx
+get 0
+call 1
+drop
+.l7
+.l5
+push 10
+dup
+send
+push 0
+ret
+.main
+resn 2
+push 0
+dup
+set 0
+push 10
+dup
+set 1
+.loop2
+get 0
+push 5
+cmplt
+jumpf l8
+.loop4
+get 1
+push 7
+cmpgt
+jumpf l10
+prep print
+get 1
+call 1
+drop
+get 1
+push 1
+sub
+dup
+set 1
+drop
+jump l11
+.l10
+jump loop5
+.l11
+jump loop4
+.loop5
+prep print
+get 0
+call 1
+drop
+get 0
+push 1
+add
+dup
+set 0
+drop
+jump l9
+.l8
+jump loop3
+.l9
+jump loop2
+.loop3
+push 0
+ret
+push 0
+ret
+.start
+prep main
+call 0
+halt</t>
+  </si>
+  <si>
+    <t>10
+9
+8
+0
+1
+2
+3
+4</t>
+  </si>
+  <si>
+    <t>Boucle "For Imbriquée"</t>
+  </si>
+  <si>
+    <t>tesForImbriq</t>
+  </si>
+  <si>
+    <t>#include&lt;stdlib&gt;
+#include&lt;stdio&gt;
+function main()
+{
+	var i;
+	var j;
+	for (i = 0; i &lt; 5; i = i + 1)
+	{
+		print(i);
+		for (j = 10; j &gt; 7; j = j - 1)
+		{
+			print(j);
+		}
+	}
+	return 0;
+}</t>
+  </si>
+  <si>
+    <t>resn 0
+.pow
+resn 2
+get 0
+dup
+set 3
+get 1
+push 1
+sub
+dup
+set 2
+.loop0
+get 2
+push 0
+cmpgt
+jumpf l0
+get 3
+get 0
+mul
+dup
+set 3
+drop
+get 2
+push 1
+sub
+dup
+set 2
+jump l1
+.l0
+jump loop1
+.l1
+jump loop0
+.loop1
+get 3
+ret
+push 0
+ret
+.printx
+resn 1
+get 0
+push 0
+cmpne
+jumpf l2
+prep printx
+get 0
+push 10
+div
+call 1
+drop
+get 0
+push 10
+mod
+push 48
+add
+dup
+set 1
+drop
+get 1
+dup
+send
+.l2
+push 0
+ret
+.print
+resn 0
+get 0
+push 0
+cmpeq
+jumpf l4
+push 48
+dup
+send
+jump l5
+.l4
+get 0
+push 0
+cmplt
+jumpf l6
+push 45
+dup
+send
+prep printx
+push 0
+get 0
+sub
+call 1
+drop
+jump l7
+.l6
+prep printx
+get 0
+call 1
+drop
+.l7
+.l5
+push 10
+dup
+send
+push 0
+ret
+.main
+resn 2
+push 0
+dup
+set 0
+.loop2
+get 0
+push 5
+cmplt
+jumpf l8
+prep print
+get 0
+call 1
+drop
+push 10
+dup
+set 1
+.loop4
+get 1
+push 7
+cmpgt
+jumpf l10
+prep print
+get 1
+call 1
+drop
+get 1
+push 1
+sub
+dup
+set 1
+jump l11
+.l10
+jump loop5
+.l11
+jump loop4
+.loop5
+get 0
+push 1
+add
+dup
+set 0
+jump l9
+.l8
+jump loop3
+.l9
+jump loop2
+.loop3
+push 0
+ret
+push 0
+ret
+.start
+prep main
+call 0
+halt</t>
+  </si>
+  <si>
+    <t>0
+10
+9
+8
+1
+10
+9
+8
+2
+10
+9
+8
+3
+10
+9
+8
+4
+10
+9
+8</t>
   </si>
 </sst>
 </file>
@@ -1847,9 +2241,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1858,6 +2249,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2175,8 +2569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB24943-54CB-4B8E-8304-8E22A3B01B04}">
   <dimension ref="B3:I452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2194,280 +2588,301 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>-1</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="288" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>3</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>1</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="6">
         <v>12</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="6">
         <v>3</v>
       </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="6">
         <v>12</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="2:9" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="2:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19" spans="2:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>49</v>
+      <c r="B19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="6" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>